<commit_message>
Add into a github
</commit_message>
<xml_diff>
--- a/ipl_palyers.xlsx
+++ b/ipl_palyers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Gitt\localrepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39D5563-FC99-41C0-B727-2C4B9C0E8029}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381C7100-909E-43D6-A4A4-033FD2E2D05D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{07B14122-F205-4AE9-8E16-105E11BBF887}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="84">
   <si>
     <t>Player</t>
   </si>
@@ -679,7 +679,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,7 +798,9 @@
       <c r="C5" s="2">
         <v>4217</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="E5" s="2">
         <v>13</v>
       </c>
@@ -925,7 +927,9 @@
       <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1052,8 +1056,12 @@
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D16" s="2">
         <v>8.4</v>
       </c>
@@ -1201,7 +1209,9 @@
       <c r="D22" s="2">
         <v>8.6</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="F22" s="2" t="s">
         <v>30</v>
       </c>
@@ -1388,7 +1398,9 @@
       <c r="C30" s="2">
         <v>2000</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="E30" s="2">
         <v>8.5</v>
       </c>
@@ -1437,7 +1449,9 @@
       <c r="D32" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="F32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1453,7 +1467,9 @@
       <c r="B33" s="2">
         <v>70</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D33" s="2">
         <v>8.3000000000000007</v>
       </c>
@@ -1808,8 +1824,12 @@
       <c r="A48" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="B48" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D48" s="2">
         <v>8.3000000000000007</v>
       </c>
@@ -1972,7 +1992,9 @@
       <c r="A55" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="C55" s="2">
         <v>1000</v>
       </c>
@@ -2033,7 +2055,9 @@
       <c r="F57" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G57" s="2"/>
+      <c r="G57" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -2043,7 +2067,9 @@
       <c r="B58" s="2">
         <v>40</v>
       </c>
-      <c r="C58" s="2"/>
+      <c r="C58" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="D58" s="2">
         <v>8.3000000000000007</v>
       </c>

</xml_diff>